<commit_message>
add nama bu heli di ttd
</commit_message>
<xml_diff>
--- a/templates/mm/bon.xlsx
+++ b/templates/mm/bon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\latihanupi\generate\server\public\xlsx\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fikriymnn/Documents/lki_upi_backend/templates/mm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF01CCDD-FD3F-426E-A7B7-E2AD9AC4D031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2F1E5A-BD22-7143-AB67-D99AAF6A55E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kuitansi (terbilang)" sheetId="8" r:id="rId1"/>
@@ -44,6 +44,19 @@
     <definedName name="trbl4">IF('Kuitansi (terbilang)'!XFD1=0,"nol",IF(TYPE('Kuitansi (terbilang)'!XFD1)=1,IF(MOD('Kuitansi (terbilang)'!XFD1,INT('Kuitansi (terbilang)'!XFD1))=0,TRIM(milyar4&amp;juta4&amp;ribu4&amp;ratus4),"ANGKA HARUS BILANGAN BULAT!"),"DATA TIDAK BOLEH BERTIPE TEKS!"))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -72,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>NO.</t>
   </si>
@@ -118,6 +131,9 @@
   <si>
     <t>${tgltanda}</t>
   </si>
+  <si>
+    <t>Dr. Heli Siti Halimatul M., M.Si</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +143,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +212,13 @@
     <font>
       <b/>
       <sz val="23"/>
+      <color indexed="8"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color indexed="8"/>
       <name val="Georgia"/>
       <family val="1"/>
@@ -382,6 +405,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,22 +438,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -924,17 +947,19 @@
   </sheetPr>
   <dimension ref="B1:CE18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="DD13" sqref="DD13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="CN12" sqref="CN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="2.7109375" style="1"/>
+    <col min="1" max="76" width="2.6640625" style="1"/>
+    <col min="77" max="77" width="11.5" style="1" customWidth="1"/>
+    <col min="78" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:83" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:83" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -946,84 +971,84 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="18" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="15" t="s">
+      <c r="AB2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="15"/>
-      <c r="BD2" s="15"/>
-      <c r="BE2" s="15"/>
-      <c r="BF2" s="15"/>
-      <c r="BG2" s="15"/>
-      <c r="BH2" s="15"/>
-      <c r="BI2" s="15"/>
-      <c r="BJ2" s="15"/>
-      <c r="BK2" s="15"/>
-      <c r="BL2" s="15"/>
-      <c r="BM2" s="15"/>
-      <c r="BN2" s="15"/>
-      <c r="BO2" s="15"/>
-      <c r="BP2" s="15"/>
-      <c r="BQ2" s="15"/>
-      <c r="BR2" s="15"/>
-      <c r="BS2" s="15"/>
-      <c r="BT2" s="15"/>
-      <c r="BU2" s="15"/>
-      <c r="BV2" s="15"/>
-      <c r="BW2" s="15"/>
-      <c r="BX2" s="15"/>
-      <c r="BY2" s="15"/>
-      <c r="BZ2" s="15"/>
-      <c r="CA2" s="15"/>
-      <c r="CB2" s="15"/>
-      <c r="CC2" s="15"/>
-      <c r="CD2" s="15"/>
-      <c r="CE2" s="15"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20"/>
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
+      <c r="CB2" s="20"/>
+      <c r="CC2" s="20"/>
+      <c r="CD2" s="20"/>
+      <c r="CE2" s="20"/>
     </row>
-    <row r="3" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1049,64 +1074,64 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
       <c r="AA3" s="12"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
-      <c r="AO3" s="15"/>
-      <c r="AP3" s="15"/>
-      <c r="AQ3" s="15"/>
-      <c r="AR3" s="15"/>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15"/>
-      <c r="AV3" s="15"/>
-      <c r="AW3" s="15"/>
-      <c r="AX3" s="15"/>
-      <c r="AY3" s="15"/>
-      <c r="AZ3" s="15"/>
-      <c r="BA3" s="15"/>
-      <c r="BB3" s="15"/>
-      <c r="BC3" s="15"/>
-      <c r="BD3" s="15"/>
-      <c r="BE3" s="15"/>
-      <c r="BF3" s="15"/>
-      <c r="BG3" s="15"/>
-      <c r="BH3" s="15"/>
-      <c r="BI3" s="15"/>
-      <c r="BJ3" s="15"/>
-      <c r="BK3" s="15"/>
-      <c r="BL3" s="15"/>
-      <c r="BM3" s="15"/>
-      <c r="BN3" s="15"/>
-      <c r="BO3" s="15"/>
-      <c r="BP3" s="15"/>
-      <c r="BQ3" s="15"/>
-      <c r="BR3" s="15"/>
-      <c r="BS3" s="15"/>
-      <c r="BT3" s="15"/>
-      <c r="BU3" s="15"/>
-      <c r="BV3" s="15"/>
-      <c r="BW3" s="15"/>
-      <c r="BX3" s="15"/>
-      <c r="BY3" s="15"/>
-      <c r="BZ3" s="15"/>
-      <c r="CA3" s="15"/>
-      <c r="CB3" s="15"/>
-      <c r="CC3" s="15"/>
-      <c r="CD3" s="15"/>
-      <c r="CE3" s="15"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="20"/>
+      <c r="BF3" s="20"/>
+      <c r="BG3" s="20"/>
+      <c r="BH3" s="20"/>
+      <c r="BI3" s="20"/>
+      <c r="BJ3" s="20"/>
+      <c r="BK3" s="20"/>
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="20"/>
+      <c r="BN3" s="20"/>
+      <c r="BO3" s="20"/>
+      <c r="BP3" s="20"/>
+      <c r="BQ3" s="20"/>
+      <c r="BR3" s="20"/>
+      <c r="BS3" s="20"/>
+      <c r="BT3" s="20"/>
+      <c r="BU3" s="20"/>
+      <c r="BV3" s="20"/>
+      <c r="BW3" s="20"/>
+      <c r="BX3" s="20"/>
+      <c r="BY3" s="20"/>
+      <c r="BZ3" s="20"/>
+      <c r="CA3" s="20"/>
+      <c r="CB3" s="20"/>
+      <c r="CC3" s="20"/>
+      <c r="CD3" s="20"/>
+      <c r="CE3" s="20"/>
     </row>
-    <row r="4" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1136,66 +1161,66 @@
       <c r="AA4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AB4" s="16" t="s">
+      <c r="AB4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="16"/>
-      <c r="AR4" s="16"/>
-      <c r="AS4" s="16"/>
-      <c r="AT4" s="16"/>
-      <c r="AU4" s="16"/>
-      <c r="AV4" s="16"/>
-      <c r="AW4" s="16"/>
-      <c r="AX4" s="16"/>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="16"/>
-      <c r="BA4" s="16"/>
-      <c r="BB4" s="16"/>
-      <c r="BC4" s="16"/>
-      <c r="BD4" s="16"/>
-      <c r="BE4" s="16"/>
-      <c r="BF4" s="16"/>
-      <c r="BG4" s="16"/>
-      <c r="BH4" s="16"/>
-      <c r="BI4" s="16"/>
-      <c r="BJ4" s="16"/>
-      <c r="BK4" s="16"/>
-      <c r="BL4" s="16"/>
-      <c r="BM4" s="16"/>
-      <c r="BN4" s="16"/>
-      <c r="BO4" s="16"/>
-      <c r="BP4" s="16"/>
-      <c r="BQ4" s="16"/>
-      <c r="BR4" s="16"/>
-      <c r="BS4" s="16"/>
-      <c r="BT4" s="16"/>
-      <c r="BU4" s="16"/>
-      <c r="BV4" s="16"/>
-      <c r="BW4" s="16"/>
-      <c r="BX4" s="16"/>
-      <c r="BY4" s="16"/>
-      <c r="BZ4" s="16"/>
-      <c r="CA4" s="16"/>
-      <c r="CB4" s="16"/>
-      <c r="CC4" s="16"/>
-      <c r="CD4" s="16"/>
-      <c r="CE4" s="16"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="21"/>
+      <c r="AR4" s="21"/>
+      <c r="AS4" s="21"/>
+      <c r="AT4" s="21"/>
+      <c r="AU4" s="21"/>
+      <c r="AV4" s="21"/>
+      <c r="AW4" s="21"/>
+      <c r="AX4" s="21"/>
+      <c r="AY4" s="21"/>
+      <c r="AZ4" s="21"/>
+      <c r="BA4" s="21"/>
+      <c r="BB4" s="21"/>
+      <c r="BC4" s="21"/>
+      <c r="BD4" s="21"/>
+      <c r="BE4" s="21"/>
+      <c r="BF4" s="21"/>
+      <c r="BG4" s="21"/>
+      <c r="BH4" s="21"/>
+      <c r="BI4" s="21"/>
+      <c r="BJ4" s="21"/>
+      <c r="BK4" s="21"/>
+      <c r="BL4" s="21"/>
+      <c r="BM4" s="21"/>
+      <c r="BN4" s="21"/>
+      <c r="BO4" s="21"/>
+      <c r="BP4" s="21"/>
+      <c r="BQ4" s="21"/>
+      <c r="BR4" s="21"/>
+      <c r="BS4" s="21"/>
+      <c r="BT4" s="21"/>
+      <c r="BU4" s="21"/>
+      <c r="BV4" s="21"/>
+      <c r="BW4" s="21"/>
+      <c r="BX4" s="21"/>
+      <c r="BY4" s="21"/>
+      <c r="BZ4" s="21"/>
+      <c r="CA4" s="21"/>
+      <c r="CB4" s="21"/>
+      <c r="CC4" s="21"/>
+      <c r="CD4" s="21"/>
+      <c r="CE4" s="21"/>
     </row>
-    <row r="5" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1278,7 +1303,7 @@
       <c r="CD5" s="2"/>
       <c r="CE5" s="2"/>
     </row>
-    <row r="6" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1308,67 +1333,67 @@
       <c r="AA6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AB6" s="17" t="str">
+      <c r="AB6" s="22" t="str">
         <f>"# "&amp;PROPER(terbilang&amp;" rupiah")&amp;" #"</f>
         <v># Data Tidak Boleh Bertipe Teks! Rupiah #</v>
       </c>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="17"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="17"/>
-      <c r="AG6" s="17"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="17"/>
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="17"/>
-      <c r="AM6" s="17"/>
-      <c r="AN6" s="17"/>
-      <c r="AO6" s="17"/>
-      <c r="AP6" s="17"/>
-      <c r="AQ6" s="17"/>
-      <c r="AR6" s="17"/>
-      <c r="AS6" s="17"/>
-      <c r="AT6" s="17"/>
-      <c r="AU6" s="17"/>
-      <c r="AV6" s="17"/>
-      <c r="AW6" s="17"/>
-      <c r="AX6" s="17"/>
-      <c r="AY6" s="17"/>
-      <c r="AZ6" s="17"/>
-      <c r="BA6" s="17"/>
-      <c r="BB6" s="17"/>
-      <c r="BC6" s="17"/>
-      <c r="BD6" s="17"/>
-      <c r="BE6" s="17"/>
-      <c r="BF6" s="17"/>
-      <c r="BG6" s="17"/>
-      <c r="BH6" s="17"/>
-      <c r="BI6" s="17"/>
-      <c r="BJ6" s="17"/>
-      <c r="BK6" s="17"/>
-      <c r="BL6" s="17"/>
-      <c r="BM6" s="17"/>
-      <c r="BN6" s="17"/>
-      <c r="BO6" s="17"/>
-      <c r="BP6" s="17"/>
-      <c r="BQ6" s="17"/>
-      <c r="BR6" s="17"/>
-      <c r="BS6" s="17"/>
-      <c r="BT6" s="17"/>
-      <c r="BU6" s="17"/>
-      <c r="BV6" s="17"/>
-      <c r="BW6" s="17"/>
-      <c r="BX6" s="17"/>
-      <c r="BY6" s="17"/>
-      <c r="BZ6" s="17"/>
-      <c r="CA6" s="17"/>
-      <c r="CB6" s="17"/>
-      <c r="CC6" s="17"/>
-      <c r="CD6" s="17"/>
-      <c r="CE6" s="17"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="22"/>
+      <c r="AM6" s="22"/>
+      <c r="AN6" s="22"/>
+      <c r="AO6" s="22"/>
+      <c r="AP6" s="22"/>
+      <c r="AQ6" s="22"/>
+      <c r="AR6" s="22"/>
+      <c r="AS6" s="22"/>
+      <c r="AT6" s="22"/>
+      <c r="AU6" s="22"/>
+      <c r="AV6" s="22"/>
+      <c r="AW6" s="22"/>
+      <c r="AX6" s="22"/>
+      <c r="AY6" s="22"/>
+      <c r="AZ6" s="22"/>
+      <c r="BA6" s="22"/>
+      <c r="BB6" s="22"/>
+      <c r="BC6" s="22"/>
+      <c r="BD6" s="22"/>
+      <c r="BE6" s="22"/>
+      <c r="BF6" s="22"/>
+      <c r="BG6" s="22"/>
+      <c r="BH6" s="22"/>
+      <c r="BI6" s="22"/>
+      <c r="BJ6" s="22"/>
+      <c r="BK6" s="22"/>
+      <c r="BL6" s="22"/>
+      <c r="BM6" s="22"/>
+      <c r="BN6" s="22"/>
+      <c r="BO6" s="22"/>
+      <c r="BP6" s="22"/>
+      <c r="BQ6" s="22"/>
+      <c r="BR6" s="22"/>
+      <c r="BS6" s="22"/>
+      <c r="BT6" s="22"/>
+      <c r="BU6" s="22"/>
+      <c r="BV6" s="22"/>
+      <c r="BW6" s="22"/>
+      <c r="BX6" s="22"/>
+      <c r="BY6" s="22"/>
+      <c r="BZ6" s="22"/>
+      <c r="CA6" s="22"/>
+      <c r="CB6" s="22"/>
+      <c r="CC6" s="22"/>
+      <c r="CD6" s="22"/>
+      <c r="CE6" s="22"/>
     </row>
-    <row r="7" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1395,7 +1420,7 @@
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
     </row>
-    <row r="8" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1425,66 +1450,66 @@
       <c r="AA8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AB8" s="21" t="s">
+      <c r="AB8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="21"/>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="21"/>
-      <c r="AK8" s="21"/>
-      <c r="AL8" s="21"/>
-      <c r="AM8" s="21"/>
-      <c r="AN8" s="21"/>
-      <c r="AO8" s="21"/>
-      <c r="AP8" s="21"/>
-      <c r="AQ8" s="21"/>
-      <c r="AR8" s="21"/>
-      <c r="AS8" s="21"/>
-      <c r="AT8" s="21"/>
-      <c r="AU8" s="21"/>
-      <c r="AV8" s="21"/>
-      <c r="AW8" s="21"/>
-      <c r="AX8" s="21"/>
-      <c r="AY8" s="21"/>
-      <c r="AZ8" s="21"/>
-      <c r="BA8" s="21"/>
-      <c r="BB8" s="21"/>
-      <c r="BC8" s="21"/>
-      <c r="BD8" s="21"/>
-      <c r="BE8" s="21"/>
-      <c r="BF8" s="21"/>
-      <c r="BG8" s="21"/>
-      <c r="BH8" s="21"/>
-      <c r="BI8" s="21"/>
-      <c r="BJ8" s="21"/>
-      <c r="BK8" s="21"/>
-      <c r="BL8" s="21"/>
-      <c r="BM8" s="21"/>
-      <c r="BN8" s="21"/>
-      <c r="BO8" s="21"/>
-      <c r="BP8" s="21"/>
-      <c r="BQ8" s="21"/>
-      <c r="BR8" s="21"/>
-      <c r="BS8" s="21"/>
-      <c r="BT8" s="21"/>
-      <c r="BU8" s="21"/>
-      <c r="BV8" s="21"/>
-      <c r="BW8" s="21"/>
-      <c r="BX8" s="21"/>
-      <c r="BY8" s="21"/>
-      <c r="BZ8" s="21"/>
-      <c r="CA8" s="21"/>
-      <c r="CB8" s="21"/>
-      <c r="CC8" s="21"/>
-      <c r="CD8" s="21"/>
-      <c r="CE8" s="21"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
+      <c r="AS8" s="14"/>
+      <c r="AT8" s="14"/>
+      <c r="AU8" s="14"/>
+      <c r="AV8" s="14"/>
+      <c r="AW8" s="14"/>
+      <c r="AX8" s="14"/>
+      <c r="AY8" s="14"/>
+      <c r="AZ8" s="14"/>
+      <c r="BA8" s="14"/>
+      <c r="BB8" s="14"/>
+      <c r="BC8" s="14"/>
+      <c r="BD8" s="14"/>
+      <c r="BE8" s="14"/>
+      <c r="BF8" s="14"/>
+      <c r="BG8" s="14"/>
+      <c r="BH8" s="14"/>
+      <c r="BI8" s="14"/>
+      <c r="BJ8" s="14"/>
+      <c r="BK8" s="14"/>
+      <c r="BL8" s="14"/>
+      <c r="BM8" s="14"/>
+      <c r="BN8" s="14"/>
+      <c r="BO8" s="14"/>
+      <c r="BP8" s="14"/>
+      <c r="BQ8" s="14"/>
+      <c r="BR8" s="14"/>
+      <c r="BS8" s="14"/>
+      <c r="BT8" s="14"/>
+      <c r="BU8" s="14"/>
+      <c r="BV8" s="14"/>
+      <c r="BW8" s="14"/>
+      <c r="BX8" s="14"/>
+      <c r="BY8" s="14"/>
+      <c r="BZ8" s="14"/>
+      <c r="CA8" s="14"/>
+      <c r="CB8" s="14"/>
+      <c r="CC8" s="14"/>
+      <c r="CD8" s="14"/>
+      <c r="CE8" s="14"/>
     </row>
-    <row r="9" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1496,80 +1521,80 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="8"/>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="21"/>
-      <c r="AJ9" s="21"/>
-      <c r="AK9" s="21"/>
-      <c r="AL9" s="21"/>
-      <c r="AM9" s="21"/>
-      <c r="AN9" s="21"/>
-      <c r="AO9" s="21"/>
-      <c r="AP9" s="21"/>
-      <c r="AQ9" s="21"/>
-      <c r="AR9" s="21"/>
-      <c r="AS9" s="21"/>
-      <c r="AT9" s="21"/>
-      <c r="AU9" s="21"/>
-      <c r="AV9" s="21"/>
-      <c r="AW9" s="21"/>
-      <c r="AX9" s="21"/>
-      <c r="AY9" s="21"/>
-      <c r="AZ9" s="21"/>
-      <c r="BA9" s="21"/>
-      <c r="BB9" s="21"/>
-      <c r="BC9" s="21"/>
-      <c r="BD9" s="21"/>
-      <c r="BE9" s="21"/>
-      <c r="BF9" s="21"/>
-      <c r="BG9" s="21"/>
-      <c r="BH9" s="21"/>
-      <c r="BI9" s="21"/>
-      <c r="BJ9" s="21"/>
-      <c r="BK9" s="21"/>
-      <c r="BL9" s="21"/>
-      <c r="BM9" s="21"/>
-      <c r="BN9" s="21"/>
-      <c r="BO9" s="21"/>
-      <c r="BP9" s="21"/>
-      <c r="BQ9" s="21"/>
-      <c r="BR9" s="21"/>
-      <c r="BS9" s="21"/>
-      <c r="BT9" s="21"/>
-      <c r="BU9" s="21"/>
-      <c r="BV9" s="21"/>
-      <c r="BW9" s="21"/>
-      <c r="BX9" s="21"/>
-      <c r="BY9" s="21"/>
-      <c r="BZ9" s="21"/>
-      <c r="CA9" s="21"/>
-      <c r="CB9" s="21"/>
-      <c r="CC9" s="21"/>
-      <c r="CD9" s="21"/>
-      <c r="CE9" s="21"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="14"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="14"/>
+      <c r="AL9" s="14"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
+      <c r="AP9" s="14"/>
+      <c r="AQ9" s="14"/>
+      <c r="AR9" s="14"/>
+      <c r="AS9" s="14"/>
+      <c r="AT9" s="14"/>
+      <c r="AU9" s="14"/>
+      <c r="AV9" s="14"/>
+      <c r="AW9" s="14"/>
+      <c r="AX9" s="14"/>
+      <c r="AY9" s="14"/>
+      <c r="AZ9" s="14"/>
+      <c r="BA9" s="14"/>
+      <c r="BB9" s="14"/>
+      <c r="BC9" s="14"/>
+      <c r="BD9" s="14"/>
+      <c r="BE9" s="14"/>
+      <c r="BF9" s="14"/>
+      <c r="BG9" s="14"/>
+      <c r="BH9" s="14"/>
+      <c r="BI9" s="14"/>
+      <c r="BJ9" s="14"/>
+      <c r="BK9" s="14"/>
+      <c r="BL9" s="14"/>
+      <c r="BM9" s="14"/>
+      <c r="BN9" s="14"/>
+      <c r="BO9" s="14"/>
+      <c r="BP9" s="14"/>
+      <c r="BQ9" s="14"/>
+      <c r="BR9" s="14"/>
+      <c r="BS9" s="14"/>
+      <c r="BT9" s="14"/>
+      <c r="BU9" s="14"/>
+      <c r="BV9" s="14"/>
+      <c r="BW9" s="14"/>
+      <c r="BX9" s="14"/>
+      <c r="BY9" s="14"/>
+      <c r="BZ9" s="14"/>
+      <c r="CA9" s="14"/>
+      <c r="CB9" s="14"/>
+      <c r="CC9" s="14"/>
+      <c r="CD9" s="14"/>
+      <c r="CE9" s="14"/>
     </row>
-    <row r="10" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1581,78 +1606,78 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="22"/>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="22"/>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="22"/>
-      <c r="AG10" s="22"/>
-      <c r="AH10" s="22"/>
-      <c r="AI10" s="22"/>
-      <c r="AJ10" s="22"/>
-      <c r="AK10" s="22"/>
-      <c r="AL10" s="22"/>
-      <c r="AM10" s="22"/>
-      <c r="AN10" s="22"/>
-      <c r="AO10" s="22"/>
-      <c r="AP10" s="22"/>
-      <c r="AQ10" s="22"/>
-      <c r="AR10" s="22"/>
-      <c r="AS10" s="22"/>
-      <c r="AT10" s="22"/>
-      <c r="AU10" s="22"/>
-      <c r="AV10" s="22"/>
-      <c r="AW10" s="22"/>
-      <c r="AX10" s="22"/>
-      <c r="AY10" s="22"/>
-      <c r="AZ10" s="22"/>
-      <c r="BA10" s="22"/>
-      <c r="BB10" s="22"/>
-      <c r="BC10" s="22"/>
-      <c r="BD10" s="22"/>
-      <c r="BE10" s="22"/>
-      <c r="BF10" s="22"/>
-      <c r="BG10" s="22"/>
-      <c r="BH10" s="22"/>
-      <c r="BI10" s="22"/>
-      <c r="BJ10" s="22"/>
-      <c r="BK10" s="22"/>
-      <c r="BL10" s="22"/>
-      <c r="BM10" s="22"/>
-      <c r="BN10" s="22"/>
-      <c r="BO10" s="22"/>
-      <c r="BP10" s="22"/>
-      <c r="BQ10" s="22"/>
-      <c r="BR10" s="22"/>
-      <c r="BS10" s="22"/>
-      <c r="BT10" s="22"/>
-      <c r="BU10" s="22"/>
-      <c r="BV10" s="22"/>
-      <c r="BW10" s="22"/>
-      <c r="BX10" s="22"/>
-      <c r="BY10" s="22"/>
-      <c r="BZ10" s="22"/>
-      <c r="CA10" s="22"/>
-      <c r="CB10" s="22"/>
-      <c r="CC10" s="22"/>
-      <c r="CD10" s="22"/>
-      <c r="CE10" s="22"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
+      <c r="AI10" s="15"/>
+      <c r="AJ10" s="15"/>
+      <c r="AK10" s="15"/>
+      <c r="AL10" s="15"/>
+      <c r="AM10" s="15"/>
+      <c r="AN10" s="15"/>
+      <c r="AO10" s="15"/>
+      <c r="AP10" s="15"/>
+      <c r="AQ10" s="15"/>
+      <c r="AR10" s="15"/>
+      <c r="AS10" s="15"/>
+      <c r="AT10" s="15"/>
+      <c r="AU10" s="15"/>
+      <c r="AV10" s="15"/>
+      <c r="AW10" s="15"/>
+      <c r="AX10" s="15"/>
+      <c r="AY10" s="15"/>
+      <c r="AZ10" s="15"/>
+      <c r="BA10" s="15"/>
+      <c r="BB10" s="15"/>
+      <c r="BC10" s="15"/>
+      <c r="BD10" s="15"/>
+      <c r="BE10" s="15"/>
+      <c r="BF10" s="15"/>
+      <c r="BG10" s="15"/>
+      <c r="BH10" s="15"/>
+      <c r="BI10" s="15"/>
+      <c r="BJ10" s="15"/>
+      <c r="BK10" s="15"/>
+      <c r="BL10" s="15"/>
+      <c r="BM10" s="15"/>
+      <c r="BN10" s="15"/>
+      <c r="BO10" s="15"/>
+      <c r="BP10" s="15"/>
+      <c r="BQ10" s="15"/>
+      <c r="BR10" s="15"/>
+      <c r="BS10" s="15"/>
+      <c r="BT10" s="15"/>
+      <c r="BU10" s="15"/>
+      <c r="BV10" s="15"/>
+      <c r="BW10" s="15"/>
+      <c r="BX10" s="15"/>
+      <c r="BY10" s="15"/>
+      <c r="BZ10" s="15"/>
+      <c r="CA10" s="15"/>
+      <c r="CB10" s="15"/>
+      <c r="CC10" s="15"/>
+      <c r="CD10" s="15"/>
+      <c r="CE10" s="15"/>
     </row>
-    <row r="11" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1664,78 +1689,78 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="8"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-      <c r="AG11" s="22"/>
-      <c r="AH11" s="22"/>
-      <c r="AI11" s="22"/>
-      <c r="AJ11" s="22"/>
-      <c r="AK11" s="22"/>
-      <c r="AL11" s="22"/>
-      <c r="AM11" s="22"/>
-      <c r="AN11" s="22"/>
-      <c r="AO11" s="22"/>
-      <c r="AP11" s="22"/>
-      <c r="AQ11" s="22"/>
-      <c r="AR11" s="22"/>
-      <c r="AS11" s="22"/>
-      <c r="AT11" s="22"/>
-      <c r="AU11" s="22"/>
-      <c r="AV11" s="22"/>
-      <c r="AW11" s="22"/>
-      <c r="AX11" s="22"/>
-      <c r="AY11" s="22"/>
-      <c r="AZ11" s="22"/>
-      <c r="BA11" s="22"/>
-      <c r="BB11" s="22"/>
-      <c r="BC11" s="22"/>
-      <c r="BD11" s="22"/>
-      <c r="BE11" s="22"/>
-      <c r="BF11" s="22"/>
-      <c r="BG11" s="22"/>
-      <c r="BH11" s="22"/>
-      <c r="BI11" s="22"/>
-      <c r="BJ11" s="22"/>
-      <c r="BK11" s="22"/>
-      <c r="BL11" s="22"/>
-      <c r="BM11" s="22"/>
-      <c r="BN11" s="22"/>
-      <c r="BO11" s="22"/>
-      <c r="BP11" s="22"/>
-      <c r="BQ11" s="22"/>
-      <c r="BR11" s="22"/>
-      <c r="BS11" s="22"/>
-      <c r="BT11" s="22"/>
-      <c r="BU11" s="22"/>
-      <c r="BV11" s="22"/>
-      <c r="BW11" s="22"/>
-      <c r="BX11" s="22"/>
-      <c r="BY11" s="22"/>
-      <c r="BZ11" s="22"/>
-      <c r="CA11" s="22"/>
-      <c r="CB11" s="22"/>
-      <c r="CC11" s="22"/>
-      <c r="CD11" s="22"/>
-      <c r="CE11" s="22"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="15"/>
+      <c r="AM11" s="15"/>
+      <c r="AN11" s="15"/>
+      <c r="AO11" s="15"/>
+      <c r="AP11" s="15"/>
+      <c r="AQ11" s="15"/>
+      <c r="AR11" s="15"/>
+      <c r="AS11" s="15"/>
+      <c r="AT11" s="15"/>
+      <c r="AU11" s="15"/>
+      <c r="AV11" s="15"/>
+      <c r="AW11" s="15"/>
+      <c r="AX11" s="15"/>
+      <c r="AY11" s="15"/>
+      <c r="AZ11" s="15"/>
+      <c r="BA11" s="15"/>
+      <c r="BB11" s="15"/>
+      <c r="BC11" s="15"/>
+      <c r="BD11" s="15"/>
+      <c r="BE11" s="15"/>
+      <c r="BF11" s="15"/>
+      <c r="BG11" s="15"/>
+      <c r="BH11" s="15"/>
+      <c r="BI11" s="15"/>
+      <c r="BJ11" s="15"/>
+      <c r="BK11" s="15"/>
+      <c r="BL11" s="15"/>
+      <c r="BM11" s="15"/>
+      <c r="BN11" s="15"/>
+      <c r="BO11" s="15"/>
+      <c r="BP11" s="15"/>
+      <c r="BQ11" s="15"/>
+      <c r="BR11" s="15"/>
+      <c r="BS11" s="15"/>
+      <c r="BT11" s="15"/>
+      <c r="BU11" s="15"/>
+      <c r="BV11" s="15"/>
+      <c r="BW11" s="15"/>
+      <c r="BX11" s="15"/>
+      <c r="BY11" s="15"/>
+      <c r="BZ11" s="15"/>
+      <c r="CA11" s="15"/>
+      <c r="CB11" s="15"/>
+      <c r="CC11" s="15"/>
+      <c r="CD11" s="15"/>
+      <c r="CE11" s="15"/>
     </row>
-    <row r="12" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1818,7 +1843,7 @@
       <c r="CD12" s="2"/>
       <c r="CE12" s="2"/>
     </row>
-    <row r="13" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:83" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1830,26 +1855,26 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
-      <c r="BJ13" s="25" t="s">
+      <c r="BJ13" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="BK13" s="25"/>
-      <c r="BL13" s="25"/>
-      <c r="BM13" s="25"/>
-      <c r="BN13" s="25"/>
-      <c r="BO13" s="25"/>
-      <c r="BP13" s="25"/>
-      <c r="BQ13" s="25"/>
-      <c r="BR13" s="25"/>
-      <c r="BS13" s="25"/>
-      <c r="BT13" s="25"/>
-      <c r="BU13" s="25"/>
-      <c r="BV13" s="25"/>
-      <c r="BW13" s="25"/>
-      <c r="BX13" s="25"/>
-      <c r="BY13" s="25"/>
+      <c r="BK13" s="18"/>
+      <c r="BL13" s="18"/>
+      <c r="BM13" s="18"/>
+      <c r="BN13" s="18"/>
+      <c r="BO13" s="18"/>
+      <c r="BP13" s="18"/>
+      <c r="BQ13" s="18"/>
+      <c r="BR13" s="18"/>
+      <c r="BS13" s="18"/>
+      <c r="BT13" s="18"/>
+      <c r="BU13" s="18"/>
+      <c r="BV13" s="18"/>
+      <c r="BW13" s="18"/>
+      <c r="BX13" s="18"/>
+      <c r="BY13" s="18"/>
     </row>
-    <row r="14" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1862,7 +1887,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="2:83" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:83" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1875,7 +1900,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="2:83" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:83" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1887,32 +1912,32 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
-      <c r="N16" s="23" t="s">
+      <c r="N16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="24" t="s">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="24"/>
-      <c r="AE16" s="24"/>
-      <c r="AF16" s="24"/>
-      <c r="AG16" s="24"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="17"/>
     </row>
-    <row r="17" spans="2:78" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:78" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1927,29 +1952,36 @@
       <c r="BI17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="BJ17" s="20"/>
-      <c r="BK17" s="20"/>
-      <c r="BL17" s="20"/>
-      <c r="BM17" s="20"/>
-      <c r="BN17" s="20"/>
-      <c r="BO17" s="20"/>
-      <c r="BP17" s="20"/>
-      <c r="BQ17" s="20"/>
-      <c r="BR17" s="20"/>
-      <c r="BS17" s="20"/>
-      <c r="BT17" s="20"/>
-      <c r="BU17" s="20"/>
-      <c r="BV17" s="20"/>
-      <c r="BW17" s="20"/>
-      <c r="BX17" s="20"/>
-      <c r="BY17" s="20"/>
+      <c r="BJ17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="BK17" s="25"/>
+      <c r="BL17" s="25"/>
+      <c r="BM17" s="25"/>
+      <c r="BN17" s="25"/>
+      <c r="BO17" s="25"/>
+      <c r="BP17" s="25"/>
+      <c r="BQ17" s="25"/>
+      <c r="BR17" s="25"/>
+      <c r="BS17" s="25"/>
+      <c r="BT17" s="25"/>
+      <c r="BU17" s="25"/>
+      <c r="BV17" s="25"/>
+      <c r="BW17" s="25"/>
+      <c r="BX17" s="25"/>
+      <c r="BY17" s="25"/>
       <c r="BZ17" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:78" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:78" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="AB2:CE3"/>
+    <mergeCell ref="AB4:CE4"/>
+    <mergeCell ref="AB6:CE6"/>
+    <mergeCell ref="Q2:Z2"/>
     <mergeCell ref="BJ17:BY17"/>
     <mergeCell ref="AB8:CE8"/>
     <mergeCell ref="N9:CE9"/>
@@ -1958,11 +1990,6 @@
     <mergeCell ref="N16:Q16"/>
     <mergeCell ref="R16:AG16"/>
     <mergeCell ref="BJ13:BY13"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="AB2:CE3"/>
-    <mergeCell ref="AB4:CE4"/>
-    <mergeCell ref="AB6:CE6"/>
-    <mergeCell ref="Q2:Z2"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>